<commit_message>
updated gantt, added new DB dump
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -126,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,6 +145,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -158,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -171,6 +177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -477,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +646,7 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>

</xml_diff>

<commit_message>
updated effort spent and gantt
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -485,7 +485,7 @@
   <dimension ref="A1:BN24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,7 +1026,7 @@
       <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1064,7 +1064,7 @@
       <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>

</xml_diff>

<commit_message>
updated gantt and effort spent
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiadifatta/Documents/GitHub/BiasielliCapoDifatta/ImplementationExtra/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14600"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -18,9 +13,6 @@
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -29,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>WHO</t>
   </si>
@@ -104,6 +96,9 @@
   </si>
   <si>
     <t>Need Notification Algorithm</t>
+  </si>
+  <si>
+    <t>BestTravelAlgorithm</t>
   </si>
 </sst>
 </file>
@@ -194,7 +189,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -496,19 +491,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN26"/>
+  <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" customWidth="1"/>
-    <col min="5" max="32" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="32" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.2">
@@ -926,7 +921,7 @@
       <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -959,7 +954,7 @@
     </row>
     <row r="12" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -997,10 +992,10 @@
     </row>
     <row r="13" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="2"/>
@@ -1011,12 +1006,12 @@
       <c r="I13" s="2"/>
       <c r="J13" s="8"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
@@ -1035,12 +1030,12 @@
     </row>
     <row r="14" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1049,12 +1044,12 @@
       <c r="I14" s="2"/>
       <c r="J14" s="8"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
@@ -1073,7 +1068,7 @@
     </row>
     <row r="15" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1111,12 +1106,12 @@
     </row>
     <row r="16" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1149,7 +1144,7 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -1187,9 +1182,12 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="9"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1222,7 +1220,7 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1256,6 +1254,9 @@
       <c r="AF19" s="3"/>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1276,7 +1277,7 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="5"/>
+      <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
@@ -1308,7 +1309,7 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
+      <c r="W21" s="5"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
@@ -1479,6 +1480,38 @@
       <c r="AE26" s="2"/>
       <c r="AF26" s="3"/>
     </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C1:D1"/>
@@ -1496,7 +1529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1508,7 +1541,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update GANTT & Effort Spent
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="432" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -494,19 +494,19 @@
   <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="4.140625" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" customWidth="1"/>
-    <col min="5" max="32" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
+    <col min="5" max="32" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
@@ -522,7 +522,7 @@
       </c>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -610,7 +610,7 @@
       <c r="BM2" s="6"/>
       <c r="BN2" s="6"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -648,7 +648,7 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -686,7 +686,7 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -724,7 +724,7 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -762,7 +762,7 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -800,7 +800,7 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -838,14 +838,14 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -876,7 +876,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="3"/>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -914,7 +914,7 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="3"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="AE11" s="2"/>
       <c r="AF11" s="3"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -990,7 +990,7 @@
       <c r="AE12" s="2"/>
       <c r="AF12" s="3"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1028,7 +1028,7 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="3"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1066,7 +1066,7 @@
       <c r="AE14" s="2"/>
       <c r="AF14" s="3"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1104,7 +1104,7 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1142,7 @@
       <c r="AE16" s="2"/>
       <c r="AF16" s="3"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1180,7 +1180,7 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="3"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1218,7 +1218,7 @@
       <c r="AE18" s="2"/>
       <c r="AF18" s="3"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="3"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="3"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1320,7 +1320,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1352,7 +1352,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1384,7 +1384,7 @@
       <c r="AE23" s="2"/>
       <c r="AF23" s="3"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1416,7 +1416,7 @@
       <c r="AE24" s="2"/>
       <c r="AF24" s="3"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1448,7 +1448,7 @@
       <c r="AE25" s="2"/>
       <c r="AF25" s="3"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1480,7 +1480,7 @@
       <c r="AE26" s="2"/>
       <c r="AF26" s="3"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1529,7 +1529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1541,7 +1541,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
GANTT & Effort Spent Update
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattiadifatta/Documents/GitHub/BiasielliCapoDifatta/ImplementationExtra/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14600"/>
+    <workbookView xWindow="0" yWindow="444" windowWidth="25596" windowHeight="14604"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -112,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,7 +192,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -502,19 +497,19 @@
   <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" customWidth="1"/>
     <col min="4" max="4" width="4.33203125" customWidth="1"/>
     <col min="5" max="32" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
@@ -530,7 +525,7 @@
       </c>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -618,7 +613,7 @@
       <c r="BM2" s="6"/>
       <c r="BN2" s="6"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -656,7 +651,7 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -694,7 +689,7 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -732,7 +727,7 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -770,14 +765,14 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -808,7 +803,7 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -846,7 +841,7 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -884,7 +879,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="3"/>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -922,7 +917,7 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="3"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -960,7 +955,7 @@
       <c r="AE11" s="2"/>
       <c r="AF11" s="3"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -998,7 +993,7 @@
       <c r="AE12" s="2"/>
       <c r="AF12" s="3"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1036,7 +1031,7 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="3"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1074,7 +1069,7 @@
       <c r="AE14" s="2"/>
       <c r="AF14" s="3"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1112,7 +1107,7 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1150,7 +1145,7 @@
       <c r="AE16" s="2"/>
       <c r="AF16" s="3"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1188,7 +1183,7 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="3"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1226,7 +1221,7 @@
       <c r="AE18" s="2"/>
       <c r="AF18" s="3"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1261,7 +1256,7 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="3"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1299,7 +1294,7 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="3"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1331,7 +1326,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1363,7 +1358,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1395,7 +1390,7 @@
       <c r="AE23" s="2"/>
       <c r="AF23" s="3"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1427,7 +1422,7 @@
       <c r="AE24" s="2"/>
       <c r="AF24" s="3"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1459,7 +1454,7 @@
       <c r="AE25" s="2"/>
       <c r="AF25" s="3"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1491,7 +1486,7 @@
       <c r="AE26" s="2"/>
       <c r="AF26" s="3"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1540,7 +1535,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1552,7 +1547,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
effort spent + gantt
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="444" windowWidth="25596" windowHeight="14604"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,6 @@
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>WHO</t>
   </si>
@@ -102,12 +99,15 @@
   </si>
   <si>
     <t>BestTravelAlgorithm</t>
+  </si>
+  <si>
+    <t>Desktop Client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -497,19 +497,19 @@
   <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" customWidth="1"/>
-    <col min="5" max="32" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="4.140625" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="32" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
@@ -525,7 +525,7 @@
       </c>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -613,14 +613,14 @@
       <c r="BM2" s="6"/>
       <c r="BN2" s="6"/>
     </row>
-    <row r="3" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="9"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -651,7 +651,7 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="3"/>
     </row>
-    <row r="4" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -689,7 +689,7 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="3"/>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -727,7 +727,7 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="3"/>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -765,7 +765,7 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -803,7 +803,7 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -841,7 +841,7 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="3"/>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -879,7 +879,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="3"/>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -917,7 +917,7 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="3"/>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -955,7 +955,7 @@
       <c r="AE11" s="2"/>
       <c r="AF11" s="3"/>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -993,7 +993,7 @@
       <c r="AE12" s="2"/>
       <c r="AF12" s="3"/>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1031,7 +1031,7 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="3"/>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="AE14" s="2"/>
       <c r="AF14" s="3"/>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1107,7 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:66" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1145,7 +1145,7 @@
       <c r="AE16" s="2"/>
       <c r="AF16" s="3"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1183,7 +1183,7 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="3"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1221,12 +1221,15 @@
       <c r="AE18" s="2"/>
       <c r="AF18" s="3"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1256,7 +1259,7 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="3"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1294,9 +1297,15 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="3"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+    <row r="21" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1326,7 +1335,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1358,7 +1367,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1390,7 +1399,7 @@
       <c r="AE23" s="2"/>
       <c r="AF23" s="3"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1422,7 +1431,7 @@
       <c r="AE24" s="2"/>
       <c r="AF24" s="3"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1454,7 +1463,7 @@
       <c r="AE25" s="2"/>
       <c r="AF25" s="3"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1486,7 +1495,7 @@
       <c r="AE26" s="2"/>
       <c r="AF26" s="3"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1535,7 +1544,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1547,7 +1556,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Effort Spent & GANTT Update
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>WHO</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Desktop Client</t>
+  </si>
+  <si>
+    <t>Mobile Client (Android)</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:BN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,9 +1339,15 @@
       <c r="AF21" s="3"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>

</xml_diff>

<commit_message>
updated effort spent, gantt
added dependencies .jar files
</commit_message>
<xml_diff>
--- a/ImplementationExtra/GANTT.xlsx
+++ b/ImplementationExtra/GANTT.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>WHO</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Desktop Client Day Overview</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -182,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -196,6 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -502,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,7 +1345,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="3"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1351,7 +1355,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1379,7 +1383,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1389,7 +1393,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="2"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -1456,11 +1460,17 @@
       <c r="AF24" s="3"/>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
       <c r="J25" s="8"/>

</xml_diff>